<commit_message>
Revisión y corrección del guión y escaleta cn_06_09_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion09/Escaleta_CN_06_09_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion09/Escaleta_CN_06_09_CO.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mpgarcia\Desktop\CienciasNaturales\fuentes\contenidos\grado06\guion09\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8730"/>
   </bookViews>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="269">
   <si>
     <t>Asignatura</t>
   </si>
@@ -666,9 +661,6 @@
     <t xml:space="preserve">Actividad que plantea completar un texto sobre las sustancias puras y las mezclas. </t>
   </si>
   <si>
-    <t xml:space="preserve">Refuerza tu aprendizaje: ¿Qué sabes de la clasificación de la materia?  </t>
-  </si>
-  <si>
     <t>Recurso M4A-01</t>
   </si>
   <si>
@@ -732,9 +724,6 @@
     <t xml:space="preserve">Primera evaluacion adicional </t>
   </si>
   <si>
-    <t xml:space="preserve">Segunda evaluacion adicional </t>
-  </si>
-  <si>
     <t xml:space="preserve">Evaluacion adicional para manejo del profesor </t>
   </si>
   <si>
@@ -750,9 +739,6 @@
     <t>Recurso M2A-01</t>
   </si>
   <si>
-    <t>Recurso M10A-01</t>
-  </si>
-  <si>
     <t>Las propiedades de la materia</t>
   </si>
   <si>
@@ -838,6 +824,12 @@
   </si>
   <si>
     <t>Evalúa tus conocimientos sobre el tema La materia y sus propiedades</t>
+  </si>
+  <si>
+    <t>Recurso M101A-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ¿Qué sabes de la clasificación de la materia?  </t>
   </si>
 </sst>
 </file>
@@ -1831,7 +1823,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1841,8 +1833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F29" sqref="A29:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1981,7 +1973,7 @@
         <v>148</v>
       </c>
       <c r="J3" s="22" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="K3" s="27" t="s">
         <v>70</v>
@@ -2031,7 +2023,7 @@
       <c r="E4" s="17"/>
       <c r="F4" s="18"/>
       <c r="G4" s="34" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H4" s="24">
         <v>2</v>
@@ -2088,7 +2080,7 @@
         <v>145</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F5" s="18" t="s">
         <v>155</v>
@@ -2103,7 +2095,7 @@
         <v>157</v>
       </c>
       <c r="J5" s="25" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="K5" s="29" t="s">
         <v>70</v>
@@ -2151,10 +2143,10 @@
         <v>145</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="G6" s="47" t="s">
         <v>165</v>
@@ -2166,7 +2158,7 @@
         <v>166</v>
       </c>
       <c r="J6" s="25" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="K6" s="29" t="s">
         <v>69</v>
@@ -2212,10 +2204,10 @@
         <v>145</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="G7" s="23" t="s">
         <v>171</v>
@@ -2273,13 +2265,13 @@
         <v>145</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F8" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="G8" s="23" t="s">
         <v>248</v>
-      </c>
-      <c r="G8" s="23" t="s">
-        <v>251</v>
       </c>
       <c r="H8" s="21">
         <v>6</v>
@@ -2288,7 +2280,7 @@
         <v>157</v>
       </c>
       <c r="J8" s="25" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="K8" s="29" t="s">
         <v>70</v>
@@ -2334,10 +2326,10 @@
         <v>145</v>
       </c>
       <c r="E9" s="56" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F9" s="57" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="G9" s="58" t="s">
         <v>177</v>
@@ -2349,7 +2341,7 @@
         <v>166</v>
       </c>
       <c r="J9" s="26" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="K9" s="60" t="s">
         <v>70</v>
@@ -2408,7 +2400,7 @@
         <v>166</v>
       </c>
       <c r="J10" s="74" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="K10" s="75" t="s">
         <v>70</v>
@@ -2619,7 +2611,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="52" t="s">
         <v>67</v>
       </c>
@@ -2630,234 +2622,232 @@
         <v>147</v>
       </c>
       <c r="D14" s="82" t="s">
-        <v>185</v>
-      </c>
-      <c r="E14" s="83" t="s">
-        <v>198</v>
-      </c>
+        <v>262</v>
+      </c>
+      <c r="E14" s="83"/>
       <c r="F14" s="57"/>
       <c r="G14" s="58" t="s">
-        <v>185</v>
+        <v>232</v>
       </c>
       <c r="H14" s="21">
         <v>12</v>
       </c>
       <c r="I14" s="59" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="J14" s="26" t="s">
-        <v>199</v>
+        <v>233</v>
       </c>
       <c r="K14" s="60" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L14" s="61" t="s">
-        <v>31</v>
-      </c>
-      <c r="M14" s="62"/>
+        <v>32</v>
+      </c>
+      <c r="M14" s="62" t="s">
+        <v>23</v>
+      </c>
       <c r="N14" s="62"/>
-      <c r="O14" s="63" t="s">
-        <v>189</v>
-      </c>
+      <c r="O14" s="63"/>
       <c r="P14" s="64" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q14" s="65" t="s">
-        <v>174</v>
+        <v>20</v>
+      </c>
+      <c r="Q14" s="65">
+        <v>6</v>
       </c>
       <c r="R14" s="65" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="S14" s="65" t="s">
-        <v>195</v>
-      </c>
-      <c r="T14" s="65" t="s">
+        <v>168</v>
+      </c>
+      <c r="T14" s="84" t="s">
+        <v>234</v>
+      </c>
+      <c r="U14" s="65" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="C15" s="54" t="s">
+        <v>147</v>
+      </c>
+      <c r="D15" s="82" t="s">
         <v>185</v>
       </c>
-      <c r="U14" s="65" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" s="81" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="67" t="s">
-        <v>146</v>
-      </c>
-      <c r="C15" s="68" t="s">
-        <v>147</v>
-      </c>
-      <c r="D15" s="69" t="s">
+      <c r="E15" s="83" t="s">
+        <v>198</v>
+      </c>
+      <c r="F15" s="57"/>
+      <c r="G15" s="58" t="s">
         <v>185</v>
-      </c>
-      <c r="E15" s="70" t="s">
-        <v>150</v>
-      </c>
-      <c r="F15" s="71"/>
-      <c r="G15" s="72" t="s">
-        <v>200</v>
       </c>
       <c r="H15" s="21">
         <v>13</v>
       </c>
-      <c r="I15" s="73" t="s">
-        <v>166</v>
-      </c>
-      <c r="J15" s="74" t="s">
-        <v>237</v>
-      </c>
-      <c r="K15" s="75" t="s">
+      <c r="I15" s="59" t="s">
+        <v>148</v>
+      </c>
+      <c r="J15" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="K15" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="L15" s="76" t="s">
-        <v>32</v>
-      </c>
-      <c r="M15" s="77" t="s">
-        <v>62</v>
-      </c>
-      <c r="N15" s="77"/>
-      <c r="O15" s="78" t="s">
-        <v>201</v>
-      </c>
-      <c r="P15" s="79" t="s">
+      <c r="L15" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="M15" s="62"/>
+      <c r="N15" s="62"/>
+      <c r="O15" s="63" t="s">
+        <v>189</v>
+      </c>
+      <c r="P15" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="Q15" s="80" t="s">
+      <c r="Q15" s="65" t="s">
         <v>174</v>
       </c>
-      <c r="R15" s="80" t="s">
+      <c r="R15" s="65" t="s">
         <v>161</v>
       </c>
-      <c r="S15" s="80" t="s">
+      <c r="S15" s="65" t="s">
         <v>195</v>
       </c>
-      <c r="T15" s="80" t="s">
-        <v>202</v>
-      </c>
-      <c r="U15" s="80" t="s">
+      <c r="T15" s="65" t="s">
+        <v>185</v>
+      </c>
+      <c r="U15" s="65" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
+    <row r="16" spans="1:21" s="81" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="67" t="s">
         <v>146</v>
       </c>
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="68" t="s">
         <v>147</v>
       </c>
-      <c r="D16" s="41" t="s">
-        <v>242</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="F16" s="16"/>
-      <c r="G16" s="49" t="s">
-        <v>204</v>
+      <c r="D16" s="69" t="s">
+        <v>185</v>
+      </c>
+      <c r="E16" s="70" t="s">
+        <v>150</v>
+      </c>
+      <c r="F16" s="71"/>
+      <c r="G16" s="72" t="s">
+        <v>200</v>
       </c>
       <c r="H16" s="24">
         <v>14</v>
       </c>
-      <c r="I16" s="21" t="s">
+      <c r="I16" s="73" t="s">
         <v>166</v>
       </c>
-      <c r="J16" s="22" t="s">
-        <v>252</v>
-      </c>
-      <c r="K16" s="27" t="s">
+      <c r="J16" s="74" t="s">
+        <v>235</v>
+      </c>
+      <c r="K16" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="L16" s="28" t="s">
+      <c r="L16" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="M16" s="33"/>
-      <c r="N16" s="33"/>
-      <c r="O16" s="33" t="s">
-        <v>227</v>
-      </c>
-      <c r="P16" s="35" t="s">
+      <c r="M16" s="77" t="s">
+        <v>62</v>
+      </c>
+      <c r="N16" s="77"/>
+      <c r="O16" s="78" t="s">
+        <v>201</v>
+      </c>
+      <c r="P16" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="Q16" s="51" t="s">
+      <c r="Q16" s="80" t="s">
         <v>174</v>
       </c>
-      <c r="R16" s="51" t="s">
+      <c r="R16" s="80" t="s">
         <v>161</v>
       </c>
-      <c r="S16" s="51" t="s">
+      <c r="S16" s="80" t="s">
         <v>195</v>
       </c>
-      <c r="T16" s="51" t="s">
-        <v>205</v>
-      </c>
-      <c r="U16" s="51" t="s">
+      <c r="T16" s="80" t="s">
+        <v>202</v>
+      </c>
+      <c r="U16" s="80" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="42" t="s">
+    <row r="17" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="48" t="s">
         <v>146</v>
       </c>
       <c r="C17" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="D17" s="43" t="s">
-        <v>242</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>257</v>
-      </c>
-      <c r="F17" s="18"/>
-      <c r="G17" s="23" t="s">
-        <v>206</v>
+      <c r="D17" s="41" t="s">
+        <v>239</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="F17" s="16"/>
+      <c r="G17" s="49" t="s">
+        <v>204</v>
       </c>
       <c r="H17" s="21">
         <v>15</v>
       </c>
-      <c r="I17" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="J17" s="25" t="s">
-        <v>259</v>
-      </c>
-      <c r="K17" s="29" t="s">
+      <c r="I17" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="J17" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="K17" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="L17" s="30" t="s">
+      <c r="L17" s="28" t="s">
         <v>32</v>
       </c>
       <c r="M17" s="33"/>
       <c r="N17" s="33"/>
-      <c r="O17" s="32" t="s">
-        <v>208</v>
+      <c r="O17" s="33" t="s">
+        <v>226</v>
       </c>
       <c r="P17" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="Q17" s="9" t="s">
+      <c r="Q17" s="51" t="s">
         <v>174</v>
       </c>
-      <c r="R17" s="9" t="s">
+      <c r="R17" s="51" t="s">
         <v>161</v>
       </c>
-      <c r="S17" s="9" t="s">
+      <c r="S17" s="51" t="s">
         <v>195</v>
       </c>
-      <c r="T17" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="U17" s="9" t="s">
+      <c r="T17" s="51" t="s">
+        <v>205</v>
+      </c>
+      <c r="U17" s="51" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="42" t="s">
         <v>67</v>
       </c>
@@ -2868,23 +2858,23 @@
         <v>147</v>
       </c>
       <c r="D18" s="43" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="23" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="H18" s="21">
         <v>16</v>
       </c>
       <c r="I18" s="24" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="J18" s="25" t="s">
-        <v>211</v>
+        <v>256</v>
       </c>
       <c r="K18" s="29" t="s">
         <v>70</v>
@@ -2895,7 +2885,7 @@
       <c r="M18" s="33"/>
       <c r="N18" s="33"/>
       <c r="O18" s="32" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="P18" s="35" t="s">
         <v>19</v>
@@ -2910,13 +2900,13 @@
         <v>195</v>
       </c>
       <c r="T18" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="U18" s="9" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="42" t="s">
         <v>67</v>
       </c>
@@ -2927,14 +2917,14 @@
         <v>147</v>
       </c>
       <c r="D19" s="43" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>214</v>
+        <v>254</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="23" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="H19" s="24">
         <v>17</v>
@@ -2943,7 +2933,7 @@
         <v>166</v>
       </c>
       <c r="J19" s="25" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="K19" s="29" t="s">
         <v>70</v>
@@ -2954,7 +2944,7 @@
       <c r="M19" s="33"/>
       <c r="N19" s="33"/>
       <c r="O19" s="32" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="P19" s="35" t="s">
         <v>19</v>
@@ -2969,530 +2959,534 @@
         <v>195</v>
       </c>
       <c r="T19" s="9" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="U19" s="9" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="52" t="s">
+    <row r="20" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="53" t="s">
+      <c r="B20" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="C20" s="54" t="s">
+      <c r="C20" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="D20" s="82" t="s">
-        <v>242</v>
-      </c>
-      <c r="E20" s="83" t="s">
-        <v>150</v>
-      </c>
-      <c r="F20" s="57"/>
-      <c r="G20" s="58" t="s">
-        <v>212</v>
+      <c r="D20" s="43" t="s">
+        <v>239</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="F20" s="18"/>
+      <c r="G20" s="23" t="s">
+        <v>214</v>
       </c>
       <c r="H20" s="21">
         <v>18</v>
       </c>
-      <c r="I20" s="59" t="s">
+      <c r="I20" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="J20" s="26" t="s">
-        <v>260</v>
-      </c>
-      <c r="K20" s="60" t="s">
-        <v>69</v>
-      </c>
-      <c r="L20" s="61" t="s">
+      <c r="J20" s="25" t="s">
+        <v>255</v>
+      </c>
+      <c r="K20" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="L20" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="M20" s="62" t="s">
-        <v>76</v>
-      </c>
-      <c r="N20" s="62"/>
-      <c r="O20" s="63"/>
-      <c r="P20" s="64" t="s">
+      <c r="M20" s="33"/>
+      <c r="N20" s="33"/>
+      <c r="O20" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="P20" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="65">
-        <v>6</v>
-      </c>
-      <c r="R20" s="65" t="s">
-        <v>167</v>
-      </c>
-      <c r="S20" s="65" t="s">
-        <v>168</v>
-      </c>
-      <c r="T20" s="84" t="s">
+      <c r="Q20" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="R20" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="S20" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="T20" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="U20" s="9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="C21" s="54" t="s">
+        <v>147</v>
+      </c>
+      <c r="D21" s="82" t="s">
         <v>239</v>
       </c>
-      <c r="U20" s="65" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" s="81" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" s="67" t="s">
-        <v>146</v>
-      </c>
-      <c r="C21" s="68" t="s">
-        <v>147</v>
-      </c>
-      <c r="D21" s="69" t="s">
-        <v>242</v>
-      </c>
-      <c r="E21" s="70" t="s">
-        <v>150</v>
-      </c>
-      <c r="F21" s="71"/>
-      <c r="G21" s="72" t="s">
-        <v>244</v>
+      <c r="E21" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="F21" s="57"/>
+      <c r="G21" s="58" t="s">
+        <v>268</v>
       </c>
       <c r="H21" s="21">
         <v>19</v>
       </c>
-      <c r="I21" s="73" t="s">
-        <v>20</v>
-      </c>
-      <c r="J21" s="74" t="s">
-        <v>238</v>
-      </c>
-      <c r="K21" s="75" t="s">
+      <c r="I21" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="J21" s="26" t="s">
+        <v>257</v>
+      </c>
+      <c r="K21" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="L21" s="76" t="s">
+      <c r="L21" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="M21" s="77" t="s">
-        <v>62</v>
-      </c>
-      <c r="N21" s="77"/>
-      <c r="O21" s="77"/>
-      <c r="P21" s="79" t="s">
+      <c r="M21" s="62" t="s">
+        <v>76</v>
+      </c>
+      <c r="N21" s="62"/>
+      <c r="O21" s="63"/>
+      <c r="P21" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="Q21" s="80">
+      <c r="Q21" s="65">
         <v>6</v>
       </c>
-      <c r="R21" s="80" t="s">
+      <c r="R21" s="65" t="s">
         <v>167</v>
       </c>
-      <c r="S21" s="80" t="s">
+      <c r="S21" s="65" t="s">
         <v>168</v>
       </c>
-      <c r="T21" s="86" t="s">
-        <v>240</v>
-      </c>
-      <c r="U21" s="80" t="s">
+      <c r="T21" s="84" t="s">
+        <v>237</v>
+      </c>
+      <c r="U21" s="65" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="38" t="s">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="B22" s="48" t="s">
+      <c r="B22" s="39" t="s">
         <v>146</v>
       </c>
       <c r="C22" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="D22" s="41" t="s">
-        <v>218</v>
-      </c>
-      <c r="E22" s="15"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="49" t="s">
-        <v>220</v>
-      </c>
-      <c r="H22" s="24">
+      <c r="D22" s="43" t="s">
+        <v>239</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="F22" s="18"/>
+      <c r="G22" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="H22" s="21">
         <v>20</v>
       </c>
-      <c r="I22" s="21" t="s">
-        <v>219</v>
-      </c>
-      <c r="J22" s="85" t="s">
-        <v>263</v>
-      </c>
-      <c r="K22" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="L22" s="28" t="s">
+      <c r="I22" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="J22" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="K22" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="L22" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="M22" s="33"/>
+      <c r="M22" s="33" t="s">
+        <v>23</v>
+      </c>
       <c r="N22" s="33"/>
-      <c r="O22" s="33" t="s">
-        <v>227</v>
-      </c>
+      <c r="O22" s="32"/>
       <c r="P22" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q22" s="51" t="s">
-        <v>174</v>
-      </c>
-      <c r="R22" s="51" t="s">
-        <v>161</v>
-      </c>
-      <c r="S22" s="51" t="s">
-        <v>162</v>
-      </c>
-      <c r="T22" s="51" t="s">
-        <v>220</v>
-      </c>
-      <c r="U22" s="51" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q22" s="9">
+        <v>6</v>
+      </c>
+      <c r="R22" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="S22" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="T22" s="36" t="s">
+        <v>216</v>
+      </c>
+      <c r="U22" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" s="81" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="67" t="s">
         <v>146</v>
       </c>
-      <c r="C23" s="40" t="s">
+      <c r="C23" s="68" t="s">
         <v>147</v>
       </c>
-      <c r="D23" s="43" t="s">
-        <v>218</v>
-      </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="23" t="s">
-        <v>261</v>
+      <c r="D23" s="69" t="s">
+        <v>239</v>
+      </c>
+      <c r="E23" s="70" t="s">
+        <v>150</v>
+      </c>
+      <c r="F23" s="71"/>
+      <c r="G23" s="72" t="s">
+        <v>241</v>
       </c>
       <c r="H23" s="21">
         <v>21</v>
       </c>
-      <c r="I23" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="J23" s="46" t="s">
-        <v>262</v>
-      </c>
-      <c r="K23" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="L23" s="30" t="s">
+      <c r="I23" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23" s="74" t="s">
+        <v>236</v>
+      </c>
+      <c r="K23" s="75" t="s">
+        <v>69</v>
+      </c>
+      <c r="L23" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="M23" s="33"/>
-      <c r="N23" s="33"/>
-      <c r="O23" s="37" t="s">
-        <v>221</v>
-      </c>
-      <c r="P23" s="35" t="s">
+      <c r="M23" s="77" t="s">
+        <v>62</v>
+      </c>
+      <c r="N23" s="77"/>
+      <c r="O23" s="77"/>
+      <c r="P23" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="R23" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="S23" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="T23" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="U23" s="9" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="42" t="s">
+      <c r="Q23" s="80">
+        <v>6</v>
+      </c>
+      <c r="R23" s="80" t="s">
+        <v>167</v>
+      </c>
+      <c r="S23" s="80" t="s">
+        <v>168</v>
+      </c>
+      <c r="T23" s="86" t="s">
+        <v>267</v>
+      </c>
+      <c r="U23" s="80" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="B24" s="39" t="s">
+      <c r="B24" s="48" t="s">
         <v>146</v>
       </c>
       <c r="C24" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="D24" s="43" t="s">
+      <c r="D24" s="41" t="s">
+        <v>217</v>
+      </c>
+      <c r="E24" s="15"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="49" t="s">
+        <v>219</v>
+      </c>
+      <c r="H24" s="24">
+        <v>22</v>
+      </c>
+      <c r="I24" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="23" t="s">
-        <v>223</v>
-      </c>
-      <c r="H24" s="21">
-        <v>22</v>
-      </c>
-      <c r="I24" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="J24" s="46" t="s">
-        <v>243</v>
-      </c>
-      <c r="K24" s="29" t="s">
+      <c r="J24" s="85" t="s">
+        <v>260</v>
+      </c>
+      <c r="K24" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="L24" s="30" t="s">
+      <c r="L24" s="28" t="s">
         <v>32</v>
       </c>
       <c r="M24" s="33"/>
       <c r="N24" s="33"/>
-      <c r="O24" s="32" t="s">
-        <v>224</v>
+      <c r="O24" s="33" t="s">
+        <v>226</v>
       </c>
       <c r="P24" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="Q24" s="9" t="s">
+      <c r="Q24" s="51" t="s">
         <v>174</v>
       </c>
-      <c r="R24" s="9" t="s">
+      <c r="R24" s="51" t="s">
         <v>161</v>
       </c>
-      <c r="S24" s="9" t="s">
+      <c r="S24" s="51" t="s">
         <v>162</v>
       </c>
-      <c r="T24" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="U24" s="9" t="s">
+      <c r="T24" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="U24" s="51" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="52" t="s">
+      <c r="A25" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="B25" s="53" t="s">
+      <c r="B25" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="C25" s="54" t="s">
+      <c r="C25" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="D25" s="82" t="s">
-        <v>218</v>
-      </c>
-      <c r="E25" s="83"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="58" t="s">
-        <v>226</v>
-      </c>
-      <c r="H25" s="24">
+      <c r="D25" s="43" t="s">
+        <v>217</v>
+      </c>
+      <c r="E25" s="17"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="23" t="s">
+        <v>258</v>
+      </c>
+      <c r="H25" s="21">
         <v>23</v>
       </c>
-      <c r="I25" s="59" t="s">
+      <c r="I25" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="J25" s="87" t="s">
-        <v>264</v>
-      </c>
-      <c r="K25" s="60" t="s">
+      <c r="J25" s="46" t="s">
+        <v>259</v>
+      </c>
+      <c r="K25" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="L25" s="61" t="s">
+      <c r="L25" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="M25" s="62"/>
-      <c r="N25" s="62"/>
-      <c r="O25" s="63" t="s">
-        <v>228</v>
-      </c>
-      <c r="P25" s="64" t="s">
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="P25" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="Q25" s="65" t="s">
+      <c r="Q25" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="R25" s="65" t="s">
+      <c r="R25" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="S25" s="65" t="s">
-        <v>195</v>
-      </c>
-      <c r="T25" s="65" t="s">
-        <v>229</v>
-      </c>
-      <c r="U25" s="65" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" s="81" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="66" t="s">
+      <c r="S25" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="T25" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="U25" s="9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="B26" s="67" t="s">
+      <c r="B26" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="C26" s="68" t="s">
+      <c r="C26" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="D26" s="69" t="s">
-        <v>218</v>
-      </c>
-      <c r="E26" s="70"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="72" t="s">
-        <v>230</v>
+      <c r="D26" s="43" t="s">
+        <v>217</v>
+      </c>
+      <c r="E26" s="17"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="23" t="s">
+        <v>222</v>
       </c>
       <c r="H26" s="21">
         <v>24</v>
       </c>
-      <c r="I26" s="73" t="s">
+      <c r="I26" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="J26" s="88" t="s">
+      <c r="J26" s="46" t="s">
+        <v>240</v>
+      </c>
+      <c r="K26" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="L26" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="M26" s="33"/>
+      <c r="N26" s="33"/>
+      <c r="O26" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="P26" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q26" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="R26" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="S26" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="T26" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="U26" s="9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="C27" s="54" t="s">
+        <v>147</v>
+      </c>
+      <c r="D27" s="82" t="s">
+        <v>217</v>
+      </c>
+      <c r="E27" s="83"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="58" t="s">
+        <v>225</v>
+      </c>
+      <c r="H27" s="24">
+        <v>25</v>
+      </c>
+      <c r="I27" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="J27" s="87" t="s">
+        <v>261</v>
+      </c>
+      <c r="K27" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="L27" s="61" t="s">
+        <v>32</v>
+      </c>
+      <c r="M27" s="62"/>
+      <c r="N27" s="62"/>
+      <c r="O27" s="63" t="s">
+        <v>227</v>
+      </c>
+      <c r="P27" s="64" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q27" s="65" t="s">
+        <v>174</v>
+      </c>
+      <c r="R27" s="65" t="s">
+        <v>161</v>
+      </c>
+      <c r="S27" s="65" t="s">
+        <v>195</v>
+      </c>
+      <c r="T27" s="65" t="s">
+        <v>228</v>
+      </c>
+      <c r="U27" s="65" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" s="81" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="67" t="s">
+        <v>146</v>
+      </c>
+      <c r="C28" s="68" t="s">
+        <v>147</v>
+      </c>
+      <c r="D28" s="69" t="s">
+        <v>217</v>
+      </c>
+      <c r="E28" s="70"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="72" t="s">
+        <v>229</v>
+      </c>
+      <c r="H28" s="21">
+        <v>26</v>
+      </c>
+      <c r="I28" s="73" t="s">
+        <v>166</v>
+      </c>
+      <c r="J28" s="88" t="s">
+        <v>230</v>
+      </c>
+      <c r="K28" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="L28" s="76" t="s">
+        <v>32</v>
+      </c>
+      <c r="M28" s="77"/>
+      <c r="N28" s="77"/>
+      <c r="O28" s="77" t="s">
+        <v>226</v>
+      </c>
+      <c r="P28" s="79" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q28" s="80" t="s">
+        <v>174</v>
+      </c>
+      <c r="R28" s="80" t="s">
+        <v>161</v>
+      </c>
+      <c r="S28" s="80" t="s">
+        <v>195</v>
+      </c>
+      <c r="T28" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="K26" s="75" t="s">
-        <v>70</v>
-      </c>
-      <c r="L26" s="76" t="s">
-        <v>32</v>
-      </c>
-      <c r="M26" s="77"/>
-      <c r="N26" s="77"/>
-      <c r="O26" s="77" t="s">
-        <v>227</v>
-      </c>
-      <c r="P26" s="79" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q26" s="80" t="s">
-        <v>174</v>
-      </c>
-      <c r="R26" s="80" t="s">
-        <v>161</v>
-      </c>
-      <c r="S26" s="80" t="s">
-        <v>195</v>
-      </c>
-      <c r="T26" s="80" t="s">
-        <v>232</v>
-      </c>
-      <c r="U26" s="80" t="s">
+      <c r="U28" s="80" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="B27" s="39" t="s">
-        <v>146</v>
-      </c>
-      <c r="C27" s="40" t="s">
-        <v>147</v>
-      </c>
-      <c r="D27" s="43" t="s">
-        <v>265</v>
-      </c>
-      <c r="E27" s="17"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="23" t="s">
-        <v>233</v>
-      </c>
-      <c r="H27" s="21">
-        <v>25</v>
-      </c>
-      <c r="I27" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="J27" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="K27" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="L27" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="M27" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="N27" s="33"/>
-      <c r="O27" s="32"/>
-      <c r="P27" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q27" s="9">
-        <v>6</v>
-      </c>
-      <c r="R27" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="S27" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="T27" s="36" t="s">
-        <v>217</v>
-      </c>
-      <c r="U27" s="9" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="B28" s="53" t="s">
-        <v>146</v>
-      </c>
-      <c r="C28" s="54" t="s">
-        <v>147</v>
-      </c>
-      <c r="D28" s="82" t="s">
-        <v>265</v>
-      </c>
-      <c r="E28" s="83"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="58" t="s">
-        <v>234</v>
-      </c>
-      <c r="H28" s="24">
-        <v>26</v>
-      </c>
-      <c r="I28" s="59" t="s">
-        <v>166</v>
-      </c>
-      <c r="J28" s="26" t="s">
-        <v>235</v>
-      </c>
-      <c r="K28" s="60" t="s">
-        <v>69</v>
-      </c>
-      <c r="L28" s="61" t="s">
-        <v>32</v>
-      </c>
-      <c r="M28" s="62" t="s">
-        <v>23</v>
-      </c>
-      <c r="N28" s="62"/>
-      <c r="O28" s="63"/>
-      <c r="P28" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q28" s="65">
-        <v>6</v>
-      </c>
-      <c r="R28" s="65" t="s">
-        <v>167</v>
-      </c>
-      <c r="S28" s="65" t="s">
-        <v>168</v>
-      </c>
-      <c r="T28" s="84" t="s">
-        <v>236</v>
-      </c>
-      <c r="U28" s="65" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A29" s="38" t="s">
         <v>67</v>
       </c>
@@ -3503,12 +3497,12 @@
         <v>147</v>
       </c>
       <c r="D29" s="41" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E29" s="15"/>
       <c r="F29" s="16"/>
       <c r="G29" s="49" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="H29" s="21">
         <v>27</v>
@@ -3517,7 +3511,7 @@
         <v>166</v>
       </c>
       <c r="J29" s="49" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="K29" s="27" t="s">
         <v>69</v>
@@ -3548,12 +3542,12 @@
         <v>147</v>
       </c>
       <c r="D30" s="43" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="18"/>
       <c r="G30" s="23" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H30" s="21">
         <v>28</v>
@@ -3562,7 +3556,7 @@
         <v>166</v>
       </c>
       <c r="J30" s="25" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="K30" s="29" t="s">
         <v>69</v>
@@ -3588,7 +3582,7 @@
         <v>168</v>
       </c>
       <c r="T30" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="U30" s="9" t="s">
         <v>170</v>
@@ -3605,12 +3599,12 @@
         <v>147</v>
       </c>
       <c r="D31" s="69" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E31" s="70"/>
       <c r="F31" s="71"/>
       <c r="G31" s="92" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="H31" s="24">
         <v>29</v>
@@ -3619,7 +3613,7 @@
         <v>166</v>
       </c>
       <c r="J31" s="74" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="K31" s="75" t="s">
         <v>70</v>
@@ -5049,6 +5043,11 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="M1:N1"/>
@@ -5064,11 +5063,6 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
escaleta CN_06_09_CO cambio de nombre recurso
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion09/Escaleta_CN_06_09_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion09/Escaleta_CN_06_09_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MIS DOCUMENTOS\Desktop\CienciasNaturales\fuentes\contenidos\grado06\guion09\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8730"/>
   </bookViews>
@@ -23,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="270">
   <si>
     <t>Asignatura</t>
   </si>
@@ -830,6 +835,9 @@
   </si>
   <si>
     <t xml:space="preserve"> ¿Qué sabes de la clasificación de la materia?  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segunda evaluacion adicional </t>
   </si>
 </sst>
 </file>
@@ -1823,7 +1831,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1833,8 +1841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F29" sqref="A29:XFD30"/>
+    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3101,7 +3109,7 @@
       </c>
       <c r="F22" s="18"/>
       <c r="G22" s="23" t="s">
-        <v>232</v>
+        <v>269</v>
       </c>
       <c r="H22" s="21">
         <v>20</v>
@@ -5043,11 +5051,6 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="M1:N1"/>
@@ -5063,6 +5066,11 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Escaleta y guion CN_06_09_CO y CN_06_11_CO
Documentos enviados a jhon por correo
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion09/Escaleta_CN_06_09_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion09/Escaleta_CN_06_09_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MIS DOCUMENTOS\Desktop\CienciasNaturales\fuentes\contenidos\grado06\guion09\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Dropbox\ASEGURESE\PLANETA\QUIMICA\CN_06_09_CO\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="269">
   <si>
     <t>Asignatura</t>
   </si>
@@ -489,9 +489,6 @@
     <t>no</t>
   </si>
   <si>
-    <t xml:space="preserve">Actividades sobre las propiedades de la mateia </t>
-  </si>
-  <si>
     <t xml:space="preserve">Cambiar propiedades por carcateristicas  y elemento por objeto </t>
   </si>
   <si>
@@ -546,9 +543,6 @@
     <t xml:space="preserve">La densidad </t>
   </si>
   <si>
-    <t>Actividades para poner en práctica lo aprendido de la densidad</t>
-  </si>
-  <si>
     <t xml:space="preserve">ninguno </t>
   </si>
   <si>
@@ -594,24 +588,15 @@
     <t xml:space="preserve">¿Qué sabes sobre las propiedades de sólidos, líquidos y gases? </t>
   </si>
   <si>
-    <t xml:space="preserve">Actividades que plantean afirmaciones sobre las propiedades de la materia. </t>
-  </si>
-  <si>
     <t>En la ficha de profesor y alumno cambiar alumnos por estudiantes</t>
   </si>
   <si>
     <t xml:space="preserve">El estado plasma </t>
   </si>
   <si>
-    <t xml:space="preserve">Reconoce el estado de la materia. </t>
-  </si>
-  <si>
     <t xml:space="preserve">No </t>
   </si>
   <si>
-    <t xml:space="preserve">Actividad que permite asociar distintas sustancias con su estado de la materia. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Elimnar  del pantallazo en el encabezado la palabra (de agregación) y de las opciones (fuego) </t>
   </si>
   <si>
@@ -642,9 +627,6 @@
     <t xml:space="preserve">Las sustancias puras </t>
   </si>
   <si>
-    <t xml:space="preserve">Identifica los elementos químicos.   </t>
-  </si>
-  <si>
     <t>Identifica los elementos químicos</t>
   </si>
   <si>
@@ -663,9 +645,6 @@
     <t>¿Qué sabes sobre las sustancias puras y las mezclas?</t>
   </si>
   <si>
-    <t xml:space="preserve">Actividad que plantea completar un texto sobre las sustancias puras y las mezclas. </t>
-  </si>
-  <si>
     <t>Recurso M4A-01</t>
   </si>
   <si>
@@ -705,9 +684,6 @@
     <t>Competencias: determinación de la masa, el volumen y la densidad</t>
   </si>
   <si>
-    <t xml:space="preserve">Competencias: estudio del proceso de solidificación de la materia. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Ninguno </t>
   </si>
   <si>
@@ -720,27 +696,12 @@
     <t xml:space="preserve">Competencias: observación de técnicas para separar mezclas </t>
   </si>
   <si>
-    <t>Actividad que propone un experimento para aprender a separar diferentes tipos de mezclas mediante técnicas de separación.</t>
-  </si>
-  <si>
     <t>Competencias: observación de técnicas para separar mezclas</t>
   </si>
   <si>
-    <t xml:space="preserve">Primera evaluacion adicional </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Evaluacion adicional para manejo del profesor </t>
-  </si>
-  <si>
     <t>Recurso M4A-03</t>
   </si>
   <si>
-    <t>Actividad para repasar conceptos de los estados de la materia</t>
-  </si>
-  <si>
-    <t>Actividades para repasar conceptos de los métodos de separación de mezclas</t>
-  </si>
-  <si>
     <t>Recurso M2A-01</t>
   </si>
   <si>
@@ -750,18 +711,12 @@
     <t>La clasificación de la materia</t>
   </si>
   <si>
-    <t xml:space="preserve">Actividad que propone un experimento para desarrollar destrezas para determinar la masa, el volumen y la densidad de diferentes objetos.  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Refuerza tu aprendizaje: Los métodos de separación de mezclas   </t>
   </si>
   <si>
     <t xml:space="preserve">Banco de actividades: La materia y sus propiedades </t>
   </si>
   <si>
-    <t>Motor que incluye preguntas de respuesta abierta del tema La materia y  sus propiedades</t>
-  </si>
-  <si>
     <t>Las propiedades generales de la materia</t>
   </si>
   <si>
@@ -786,18 +741,12 @@
     <t xml:space="preserve">Actividades para poner en práctica lo aprendido de la masa y el volumen </t>
   </si>
   <si>
-    <t>Secuencia de imágenes que permite para comprender qué es la densidad y cómo se mide</t>
-  </si>
-  <si>
     <t>Actividad que plantea completar un texto sobre las propiedades físicas de la materia</t>
   </si>
   <si>
     <t>Las mezclas</t>
   </si>
   <si>
-    <t xml:space="preserve">Actividad para  asociar imágenes de técnicas de separación de mezclas con su nombre y características </t>
-  </si>
-  <si>
     <t>Animación que describe la naturaleza y composición de una disolución</t>
   </si>
   <si>
@@ -810,9 +759,6 @@
     <t xml:space="preserve">Actividad que propone un experimento para observar y comprender los cambios de estado entre sólido, líquido y gas  </t>
   </si>
   <si>
-    <t xml:space="preserve">Actividad que propone desarrollar destrezas para aprender a identificar cuáles son  las propiedades según el estado de la materia  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Actividad que propone un experimento para identificar el proceso de solidificación de la materia a través de la observación de diferentes situaciones </t>
   </si>
   <si>
@@ -837,7 +783,58 @@
     <t xml:space="preserve"> ¿Qué sabes de la clasificación de la materia?  </t>
   </si>
   <si>
-    <t xml:space="preserve">Segunda evaluacion adicional </t>
+    <t>Secuencia de imágenes que permite comprender qué es la densidad y cómo se mide</t>
+  </si>
+  <si>
+    <t>Actividades que plantean afirmaciones sobre las propiedades de la materia</t>
+  </si>
+  <si>
+    <t>Actividad que permite asociar distintas sustancias con su estado de la materia</t>
+  </si>
+  <si>
+    <t>¿Qué tanto sabes de los estados de la materia?</t>
+  </si>
+  <si>
+    <t>Actividades sobre los estados de la materia</t>
+  </si>
+  <si>
+    <t>Actividad que plantea completar un texto sobre las sustancias puras y las mezclas</t>
+  </si>
+  <si>
+    <t>Actividades sobre los métodos de separación de mezclas</t>
+  </si>
+  <si>
+    <t>Actividad que propone un experimento para desarrollar destrezas para determinar la masa, el volumen y la densidad de diferentes objetos</t>
+  </si>
+  <si>
+    <t>Actividad que propone un experimento para aprender a separar diferentes tipos de mezclas mediante técnicas de separación</t>
+  </si>
+  <si>
+    <t>Las características de los estados físicos de la materia</t>
+  </si>
+  <si>
+    <t>Actividad que plantea preguntas sobre las propiedades de la materia</t>
+  </si>
+  <si>
+    <t>Las mezclas y las técnicas de separación</t>
+  </si>
+  <si>
+    <t>Actividad que permite evaluar los conocimientos sobre las mezclas y técnicas de separación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividades sobre las propiedades de la materia </t>
+  </si>
+  <si>
+    <t>Actividades para poner en práctica lo aprendido sobre la densidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad para asociar imágenes de técnicas de separación de mezclas con su nombre y características </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad que propone desarrollar destrezas para aprender a identificar cuáles son las propiedades según el estado de la materia  </t>
+  </si>
+  <si>
+    <t>Banco de actividades del tema La materia y sus propiedades</t>
   </si>
 </sst>
 </file>
@@ -880,7 +877,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -929,6 +926,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="37">
     <border>
@@ -1388,7 +1391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1465,9 +1468,6 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1558,6 +1558,45 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1841,8 +1880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="R15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1869,92 +1908,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="98" t="s">
+      <c r="B1" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="98" t="s">
+      <c r="C1" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="98" t="s">
+      <c r="D1" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="98" t="s">
+      <c r="E1" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="98" t="s">
+      <c r="F1" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="98" t="s">
+      <c r="G1" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="98" t="s">
+      <c r="H1" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="98" t="s">
+      <c r="I1" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="98" t="s">
+      <c r="J1" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="104" t="s">
+      <c r="K1" s="103" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="102" t="s">
+      <c r="L1" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="100" t="s">
+      <c r="M1" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="100"/>
-      <c r="O1" s="98" t="s">
+      <c r="N1" s="99"/>
+      <c r="O1" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="98" t="s">
+      <c r="P1" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="98" t="s">
+      <c r="Q1" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="98" t="s">
+      <c r="R1" s="97" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="98" t="s">
+      <c r="S1" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="98" t="s">
+      <c r="T1" s="97" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="98" t="s">
+      <c r="U1" s="97" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="10" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="99"/>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="105"/>
-      <c r="L2" s="103"/>
+      <c r="A2" s="98"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="102"/>
       <c r="M2" s="14"/>
       <c r="N2" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="O2" s="99"/>
-      <c r="P2" s="99"/>
-      <c r="Q2" s="101"/>
-      <c r="R2" s="101"/>
-      <c r="S2" s="101"/>
-      <c r="T2" s="101"/>
-      <c r="U2" s="101"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="98"/>
+      <c r="Q2" s="100"/>
+      <c r="R2" s="100"/>
+      <c r="S2" s="100"/>
+      <c r="T2" s="100"/>
+      <c r="U2" s="100"/>
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
@@ -1981,7 +2020,7 @@
         <v>148</v>
       </c>
       <c r="J3" s="22" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="K3" s="27" t="s">
         <v>70</v>
@@ -1994,7 +2033,7 @@
         <v>34</v>
       </c>
       <c r="O3" s="33" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="P3" s="35" t="s">
         <v>19</v>
@@ -2003,16 +2042,16 @@
         <v>5</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S3" s="9" t="s">
         <v>145</v>
       </c>
       <c r="T3" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="U3" s="9" t="s">
         <v>159</v>
-      </c>
-      <c r="U3" s="9" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2031,7 +2070,7 @@
       <c r="E4" s="17"/>
       <c r="F4" s="18"/>
       <c r="G4" s="34" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="H4" s="24">
         <v>2</v>
@@ -2040,7 +2079,7 @@
         <v>152</v>
       </c>
       <c r="J4" s="25" t="s">
-        <v>153</v>
+        <v>264</v>
       </c>
       <c r="K4" s="29" t="s">
         <v>70</v>
@@ -2053,25 +2092,25 @@
       </c>
       <c r="N4" s="33"/>
       <c r="O4" s="32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="P4" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="R4" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="S4" s="9" t="s">
         <v>161</v>
-      </c>
-      <c r="S4" s="9" t="s">
-        <v>162</v>
       </c>
       <c r="T4" s="9" t="s">
         <v>151</v>
       </c>
       <c r="U4" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2088,22 +2127,22 @@
         <v>145</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="F5" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="G5" s="34" t="s">
         <v>155</v>
-      </c>
-      <c r="G5" s="34" t="s">
-        <v>156</v>
       </c>
       <c r="H5" s="21">
         <v>3</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J5" s="25" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="K5" s="29" t="s">
         <v>70</v>
@@ -2116,7 +2155,7 @@
         <v>34</v>
       </c>
       <c r="O5" s="37" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="P5" s="35" t="s">
         <v>19</v>
@@ -2125,16 +2164,16 @@
         <v>5</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S5" s="9" t="s">
         <v>145</v>
       </c>
       <c r="T5" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="U5" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -2151,22 +2190,22 @@
         <v>145</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="G6" s="47" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H6" s="21">
         <v>4</v>
       </c>
       <c r="I6" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J6" s="25" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="K6" s="29" t="s">
         <v>69</v>
@@ -2180,22 +2219,22 @@
       <c r="N6" s="33"/>
       <c r="O6" s="32"/>
       <c r="P6" s="35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Q6" s="9">
         <v>6</v>
       </c>
       <c r="R6" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="S6" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="S6" s="9" t="s">
+      <c r="T6" s="36" t="s">
         <v>168</v>
       </c>
-      <c r="T6" s="36" t="s">
+      <c r="U6" s="9" t="s">
         <v>169</v>
-      </c>
-      <c r="U6" s="9" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -2212,22 +2251,22 @@
         <v>145</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H7" s="24">
         <v>5</v>
       </c>
       <c r="I7" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J7" s="25" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="K7" s="29" t="s">
         <v>70</v>
@@ -2238,25 +2277,25 @@
       <c r="M7" s="33"/>
       <c r="N7" s="33"/>
       <c r="O7" s="32" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="P7" s="35" t="s">
         <v>148</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="R7" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="S7" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="S7" s="9" t="s">
+      <c r="T7" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="U7" s="9" t="s">
         <v>162</v>
-      </c>
-      <c r="T7" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="U7" s="9" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2273,22 +2312,22 @@
         <v>145</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="H8" s="21">
         <v>6</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J8" s="25" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K8" s="29" t="s">
         <v>70</v>
@@ -2299,7 +2338,7 @@
       <c r="M8" s="33"/>
       <c r="N8" s="33"/>
       <c r="O8" s="32" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="P8" s="35" t="s">
         <v>19</v>
@@ -2308,197 +2347,197 @@
         <v>5</v>
       </c>
       <c r="R8" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S8" s="9" t="s">
         <v>145</v>
       </c>
       <c r="T8" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U8" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="52" t="s">
         <v>146</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="53" t="s">
         <v>147</v>
       </c>
-      <c r="D9" s="55" t="s">
+      <c r="D9" s="54" t="s">
         <v>145</v>
       </c>
-      <c r="E9" s="56" t="s">
-        <v>238</v>
-      </c>
-      <c r="F9" s="57" t="s">
-        <v>245</v>
-      </c>
-      <c r="G9" s="58" t="s">
-        <v>177</v>
+      <c r="E9" s="55" t="s">
+        <v>225</v>
+      </c>
+      <c r="F9" s="56" t="s">
+        <v>230</v>
+      </c>
+      <c r="G9" s="57" t="s">
+        <v>175</v>
       </c>
       <c r="H9" s="21">
         <v>7</v>
       </c>
-      <c r="I9" s="59" t="s">
-        <v>166</v>
+      <c r="I9" s="58" t="s">
+        <v>165</v>
       </c>
       <c r="J9" s="26" t="s">
-        <v>253</v>
-      </c>
-      <c r="K9" s="60" t="s">
+        <v>237</v>
+      </c>
+      <c r="K9" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="L9" s="61" t="s">
+      <c r="L9" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="62"/>
-      <c r="N9" s="62"/>
-      <c r="O9" s="63" t="s">
-        <v>173</v>
-      </c>
-      <c r="P9" s="64" t="s">
+      <c r="M9" s="61"/>
+      <c r="N9" s="61"/>
+      <c r="O9" s="62" t="s">
+        <v>171</v>
+      </c>
+      <c r="P9" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" s="65">
+      <c r="Q9" s="64">
         <v>5</v>
       </c>
-      <c r="R9" s="65" t="s">
-        <v>158</v>
-      </c>
-      <c r="S9" s="65" t="s">
+      <c r="R9" s="64" t="s">
+        <v>157</v>
+      </c>
+      <c r="S9" s="64" t="s">
         <v>145</v>
       </c>
-      <c r="T9" s="65" t="s">
-        <v>178</v>
-      </c>
-      <c r="U9" s="65" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" s="81" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="66" t="s">
+      <c r="T9" s="64" t="s">
+        <v>176</v>
+      </c>
+      <c r="U9" s="64" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" s="80" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="66" t="s">
         <v>146</v>
       </c>
-      <c r="C10" s="68" t="s">
+      <c r="C10" s="67" t="s">
         <v>147</v>
       </c>
-      <c r="D10" s="69" t="s">
+      <c r="D10" s="68" t="s">
         <v>145</v>
       </c>
-      <c r="E10" s="70" t="s">
+      <c r="E10" s="69" t="s">
         <v>150</v>
       </c>
-      <c r="F10" s="71"/>
-      <c r="G10" s="72" t="s">
-        <v>181</v>
+      <c r="F10" s="70"/>
+      <c r="G10" s="71" t="s">
+        <v>179</v>
       </c>
       <c r="H10" s="24">
         <v>8</v>
       </c>
-      <c r="I10" s="73" t="s">
-        <v>166</v>
-      </c>
-      <c r="J10" s="74" t="s">
-        <v>250</v>
-      </c>
-      <c r="K10" s="75" t="s">
+      <c r="I10" s="72" t="s">
+        <v>165</v>
+      </c>
+      <c r="J10" s="73" t="s">
+        <v>235</v>
+      </c>
+      <c r="K10" s="74" t="s">
         <v>70</v>
       </c>
-      <c r="L10" s="76" t="s">
+      <c r="L10" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="M10" s="77" t="s">
+      <c r="M10" s="76" t="s">
         <v>62</v>
       </c>
-      <c r="N10" s="77"/>
-      <c r="O10" s="78" t="s">
+      <c r="N10" s="76"/>
+      <c r="O10" s="77" t="s">
+        <v>180</v>
+      </c>
+      <c r="P10" s="78" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q10" s="79">
+        <v>5</v>
+      </c>
+      <c r="R10" s="79" t="s">
+        <v>157</v>
+      </c>
+      <c r="S10" s="79" t="s">
+        <v>145</v>
+      </c>
+      <c r="T10" s="79" t="s">
+        <v>181</v>
+      </c>
+      <c r="U10" s="79" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" s="114" customFormat="1" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="105" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="106" t="s">
+        <v>146</v>
+      </c>
+      <c r="C11" s="107" t="s">
+        <v>147</v>
+      </c>
+      <c r="D11" s="108" t="s">
+        <v>183</v>
+      </c>
+      <c r="E11" s="106" t="s">
         <v>182</v>
       </c>
-      <c r="P10" s="79" t="s">
+      <c r="F11" s="107"/>
+      <c r="G11" s="108" t="s">
+        <v>260</v>
+      </c>
+      <c r="H11" s="109">
+        <v>9</v>
+      </c>
+      <c r="I11" s="109" t="s">
+        <v>156</v>
+      </c>
+      <c r="J11" s="110" t="s">
+        <v>184</v>
+      </c>
+      <c r="K11" s="106" t="s">
+        <v>70</v>
+      </c>
+      <c r="L11" s="111" t="s">
+        <v>31</v>
+      </c>
+      <c r="M11" s="112"/>
+      <c r="N11" s="112"/>
+      <c r="O11" s="112" t="s">
+        <v>186</v>
+      </c>
+      <c r="P11" s="113" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" s="80">
+      <c r="Q11" s="111">
         <v>5</v>
       </c>
-      <c r="R10" s="80" t="s">
-        <v>158</v>
-      </c>
-      <c r="S10" s="80" t="s">
+      <c r="R11" s="111" t="s">
+        <v>157</v>
+      </c>
+      <c r="S11" s="111" t="s">
         <v>145</v>
       </c>
-      <c r="T10" s="80" t="s">
+      <c r="T11" s="111" t="s">
         <v>183</v>
       </c>
-      <c r="U10" s="80" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="48" t="s">
-        <v>146</v>
-      </c>
-      <c r="C11" s="40" t="s">
-        <v>147</v>
-      </c>
-      <c r="D11" s="41" t="s">
-        <v>185</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="49" t="s">
-        <v>185</v>
-      </c>
-      <c r="H11" s="21">
-        <v>9</v>
-      </c>
-      <c r="I11" s="21" t="s">
-        <v>157</v>
-      </c>
-      <c r="J11" s="50" t="s">
-        <v>186</v>
-      </c>
-      <c r="K11" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="L11" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="M11" s="33"/>
-      <c r="N11" s="33"/>
-      <c r="O11" s="33" t="s">
-        <v>189</v>
-      </c>
-      <c r="P11" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q11" s="51">
-        <v>5</v>
-      </c>
-      <c r="R11" s="51" t="s">
-        <v>158</v>
-      </c>
-      <c r="S11" s="51" t="s">
-        <v>145</v>
-      </c>
-      <c r="T11" s="51" t="s">
-        <v>185</v>
-      </c>
-      <c r="U11" s="51" t="s">
-        <v>160</v>
+      <c r="U11" s="111" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2512,23 +2551,23 @@
         <v>147</v>
       </c>
       <c r="D12" s="43" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F12" s="18"/>
       <c r="G12" s="23" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H12" s="21">
         <v>10</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J12" s="25" t="s">
-        <v>188</v>
+        <v>252</v>
       </c>
       <c r="K12" s="29" t="s">
         <v>70</v>
@@ -2539,25 +2578,25 @@
       <c r="M12" s="33"/>
       <c r="N12" s="33"/>
       <c r="O12" s="32" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="P12" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q12" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="R12" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="S12" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="S12" s="9" t="s">
+      <c r="T12" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="U12" s="9" t="s">
         <v>162</v>
-      </c>
-      <c r="T12" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="U12" s="9" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2571,10 +2610,10 @@
         <v>147</v>
       </c>
       <c r="D13" s="43" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F13" s="18"/>
       <c r="G13" s="23" t="s">
@@ -2584,10 +2623,10 @@
         <v>11</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="J13" s="25" t="s">
-        <v>193</v>
+        <v>253</v>
       </c>
       <c r="K13" s="29" t="s">
         <v>70</v>
@@ -2598,202 +2637,202 @@
       <c r="M13" s="33"/>
       <c r="N13" s="33"/>
       <c r="O13" s="32" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="P13" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q13" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="R13" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S13" s="9" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="T13" s="9" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="U13" s="9" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="52" t="s">
+      <c r="A14" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="53" t="s">
+      <c r="B14" s="52" t="s">
         <v>146</v>
       </c>
-      <c r="C14" s="54" t="s">
+      <c r="C14" s="53" t="s">
         <v>147</v>
       </c>
-      <c r="D14" s="82" t="s">
-        <v>262</v>
-      </c>
-      <c r="E14" s="83"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="58" t="s">
-        <v>232</v>
+      <c r="D14" s="81" t="s">
+        <v>244</v>
+      </c>
+      <c r="E14" s="82"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="57" t="s">
+        <v>254</v>
       </c>
       <c r="H14" s="21">
         <v>12</v>
       </c>
-      <c r="I14" s="59" t="s">
+      <c r="I14" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="J14" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="K14" s="59" t="s">
+        <v>69</v>
+      </c>
+      <c r="L14" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="M14" s="61" t="s">
+        <v>23</v>
+      </c>
+      <c r="N14" s="61"/>
+      <c r="O14" s="62"/>
+      <c r="P14" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q14" s="64">
+        <v>6</v>
+      </c>
+      <c r="R14" s="64" t="s">
         <v>166</v>
       </c>
-      <c r="J14" s="26" t="s">
-        <v>233</v>
-      </c>
-      <c r="K14" s="60" t="s">
-        <v>69</v>
-      </c>
-      <c r="L14" s="61" t="s">
-        <v>32</v>
-      </c>
-      <c r="M14" s="62" t="s">
-        <v>23</v>
-      </c>
-      <c r="N14" s="62"/>
-      <c r="O14" s="63"/>
-      <c r="P14" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q14" s="65">
-        <v>6</v>
-      </c>
-      <c r="R14" s="65" t="s">
+      <c r="S14" s="64" t="s">
         <v>167</v>
       </c>
-      <c r="S14" s="65" t="s">
-        <v>168</v>
-      </c>
-      <c r="T14" s="84" t="s">
-        <v>234</v>
-      </c>
-      <c r="U14" s="65" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="52" t="s">
+      <c r="T14" s="83" t="s">
+        <v>223</v>
+      </c>
+      <c r="U14" s="64" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" s="114" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="115" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="116" t="s">
         <v>146</v>
       </c>
-      <c r="C15" s="54" t="s">
+      <c r="C15" s="117" t="s">
         <v>147</v>
       </c>
-      <c r="D15" s="82" t="s">
-        <v>185</v>
-      </c>
-      <c r="E15" s="83" t="s">
-        <v>198</v>
-      </c>
-      <c r="F15" s="57"/>
-      <c r="G15" s="58" t="s">
-        <v>185</v>
-      </c>
-      <c r="H15" s="21">
+      <c r="D15" s="118" t="s">
+        <v>183</v>
+      </c>
+      <c r="E15" s="116" t="s">
+        <v>193</v>
+      </c>
+      <c r="F15" s="119"/>
+      <c r="G15" s="118" t="s">
+        <v>183</v>
+      </c>
+      <c r="H15" s="109">
         <v>13</v>
       </c>
-      <c r="I15" s="59" t="s">
+      <c r="I15" s="120" t="s">
         <v>148</v>
       </c>
-      <c r="J15" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="K15" s="60" t="s">
+      <c r="J15" s="121" t="s">
+        <v>194</v>
+      </c>
+      <c r="K15" s="116" t="s">
         <v>70</v>
       </c>
-      <c r="L15" s="61" t="s">
+      <c r="L15" s="122" t="s">
         <v>31</v>
       </c>
-      <c r="M15" s="62"/>
-      <c r="N15" s="62"/>
-      <c r="O15" s="63" t="s">
-        <v>189</v>
-      </c>
-      <c r="P15" s="64" t="s">
+      <c r="M15" s="123"/>
+      <c r="N15" s="123"/>
+      <c r="O15" s="124" t="s">
+        <v>186</v>
+      </c>
+      <c r="P15" s="125" t="s">
         <v>19</v>
       </c>
-      <c r="Q15" s="65" t="s">
-        <v>174</v>
-      </c>
-      <c r="R15" s="65" t="s">
-        <v>161</v>
-      </c>
-      <c r="S15" s="65" t="s">
+      <c r="Q15" s="122" t="s">
+        <v>172</v>
+      </c>
+      <c r="R15" s="122" t="s">
+        <v>160</v>
+      </c>
+      <c r="S15" s="122" t="s">
+        <v>190</v>
+      </c>
+      <c r="T15" s="122" t="s">
+        <v>183</v>
+      </c>
+      <c r="U15" s="122" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" s="80" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="65" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="66" t="s">
+        <v>146</v>
+      </c>
+      <c r="C16" s="67" t="s">
+        <v>147</v>
+      </c>
+      <c r="D16" s="68" t="s">
+        <v>183</v>
+      </c>
+      <c r="E16" s="69" t="s">
+        <v>150</v>
+      </c>
+      <c r="F16" s="70"/>
+      <c r="G16" s="71" t="s">
         <v>195</v>
-      </c>
-      <c r="T15" s="65" t="s">
-        <v>185</v>
-      </c>
-      <c r="U15" s="65" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" s="81" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="67" t="s">
-        <v>146</v>
-      </c>
-      <c r="C16" s="68" t="s">
-        <v>147</v>
-      </c>
-      <c r="D16" s="69" t="s">
-        <v>185</v>
-      </c>
-      <c r="E16" s="70" t="s">
-        <v>150</v>
-      </c>
-      <c r="F16" s="71"/>
-      <c r="G16" s="72" t="s">
-        <v>200</v>
       </c>
       <c r="H16" s="24">
         <v>14</v>
       </c>
-      <c r="I16" s="73" t="s">
-        <v>166</v>
-      </c>
-      <c r="J16" s="74" t="s">
-        <v>235</v>
-      </c>
-      <c r="K16" s="75" t="s">
+      <c r="I16" s="72" t="s">
+        <v>165</v>
+      </c>
+      <c r="J16" s="73" t="s">
+        <v>255</v>
+      </c>
+      <c r="K16" s="74" t="s">
         <v>70</v>
       </c>
-      <c r="L16" s="76" t="s">
+      <c r="L16" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="M16" s="77" t="s">
+      <c r="M16" s="76" t="s">
         <v>62</v>
       </c>
-      <c r="N16" s="77"/>
-      <c r="O16" s="78" t="s">
-        <v>201</v>
-      </c>
-      <c r="P16" s="79" t="s">
+      <c r="N16" s="76"/>
+      <c r="O16" s="77" t="s">
+        <v>196</v>
+      </c>
+      <c r="P16" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="Q16" s="80" t="s">
-        <v>174</v>
-      </c>
-      <c r="R16" s="80" t="s">
-        <v>161</v>
-      </c>
-      <c r="S16" s="80" t="s">
-        <v>195</v>
-      </c>
-      <c r="T16" s="80" t="s">
-        <v>202</v>
-      </c>
-      <c r="U16" s="80" t="s">
+      <c r="Q16" s="79" t="s">
+        <v>172</v>
+      </c>
+      <c r="R16" s="79" t="s">
+        <v>160</v>
+      </c>
+      <c r="S16" s="79" t="s">
+        <v>190</v>
+      </c>
+      <c r="T16" s="79" t="s">
         <v>197</v>
+      </c>
+      <c r="U16" s="79" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2807,23 +2846,23 @@
         <v>147</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="F17" s="16"/>
       <c r="G17" s="49" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="H17" s="21">
         <v>15</v>
       </c>
       <c r="I17" s="21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J17" s="22" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="K17" s="27" t="s">
         <v>70</v>
@@ -2834,25 +2873,25 @@
       <c r="M17" s="33"/>
       <c r="N17" s="33"/>
       <c r="O17" s="33" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="P17" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="Q17" s="51" t="s">
-        <v>174</v>
-      </c>
-      <c r="R17" s="51" t="s">
-        <v>161</v>
-      </c>
-      <c r="S17" s="51" t="s">
-        <v>195</v>
-      </c>
-      <c r="T17" s="51" t="s">
-        <v>205</v>
-      </c>
-      <c r="U17" s="51" t="s">
-        <v>197</v>
+      <c r="Q17" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="R17" s="50" t="s">
+        <v>160</v>
+      </c>
+      <c r="S17" s="50" t="s">
+        <v>190</v>
+      </c>
+      <c r="T17" s="50" t="s">
+        <v>199</v>
+      </c>
+      <c r="U17" s="50" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2866,23 +2905,23 @@
         <v>147</v>
       </c>
       <c r="D18" s="43" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="23" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="H18" s="21">
         <v>16</v>
       </c>
       <c r="I18" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J18" s="25" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
       <c r="K18" s="29" t="s">
         <v>70</v>
@@ -2893,25 +2932,25 @@
       <c r="M18" s="33"/>
       <c r="N18" s="33"/>
       <c r="O18" s="32" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="P18" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q18" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="R18" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S18" s="9" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="T18" s="9" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="U18" s="9" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -2925,23 +2964,23 @@
         <v>147</v>
       </c>
       <c r="D19" s="43" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="23" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="H19" s="24">
         <v>17</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J19" s="25" t="s">
-        <v>211</v>
+        <v>256</v>
       </c>
       <c r="K19" s="29" t="s">
         <v>70</v>
@@ -2952,28 +2991,28 @@
       <c r="M19" s="33"/>
       <c r="N19" s="33"/>
       <c r="O19" s="32" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="P19" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q19" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="R19" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S19" s="9" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="T19" s="9" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="U19" s="9" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="42" t="s">
         <v>67</v>
       </c>
@@ -2984,23 +3023,23 @@
         <v>147</v>
       </c>
       <c r="D20" s="43" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="F20" s="18"/>
       <c r="G20" s="23" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="H20" s="21">
         <v>18</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J20" s="25" t="s">
-        <v>255</v>
+        <v>266</v>
       </c>
       <c r="K20" s="29" t="s">
         <v>70</v>
@@ -3011,84 +3050,84 @@
       <c r="M20" s="33"/>
       <c r="N20" s="33"/>
       <c r="O20" s="32" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="P20" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q20" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="R20" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S20" s="9" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="T20" s="9" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="U20" s="9" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="52" t="s">
+      <c r="A21" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="B21" s="53" t="s">
+      <c r="B21" s="52" t="s">
         <v>146</v>
       </c>
-      <c r="C21" s="54" t="s">
+      <c r="C21" s="53" t="s">
         <v>147</v>
       </c>
-      <c r="D21" s="82" t="s">
-        <v>239</v>
+      <c r="D21" s="81" t="s">
+        <v>226</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>213</v>
-      </c>
-      <c r="F21" s="57"/>
-      <c r="G21" s="58" t="s">
-        <v>268</v>
+        <v>206</v>
+      </c>
+      <c r="F21" s="56"/>
+      <c r="G21" s="57" t="s">
+        <v>250</v>
       </c>
       <c r="H21" s="21">
         <v>19</v>
       </c>
-      <c r="I21" s="59" t="s">
+      <c r="I21" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="J21" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="K21" s="59" t="s">
+        <v>69</v>
+      </c>
+      <c r="L21" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="M21" s="61" t="s">
+        <v>76</v>
+      </c>
+      <c r="N21" s="61"/>
+      <c r="O21" s="62"/>
+      <c r="P21" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q21" s="64">
+        <v>6</v>
+      </c>
+      <c r="R21" s="64" t="s">
         <v>166</v>
       </c>
-      <c r="J21" s="26" t="s">
-        <v>257</v>
-      </c>
-      <c r="K21" s="60" t="s">
-        <v>69</v>
-      </c>
-      <c r="L21" s="61" t="s">
-        <v>32</v>
-      </c>
-      <c r="M21" s="62" t="s">
-        <v>76</v>
-      </c>
-      <c r="N21" s="62"/>
-      <c r="O21" s="63"/>
-      <c r="P21" s="64" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q21" s="65">
-        <v>6</v>
-      </c>
-      <c r="R21" s="65" t="s">
+      <c r="S21" s="64" t="s">
         <v>167</v>
       </c>
-      <c r="S21" s="65" t="s">
-        <v>168</v>
-      </c>
-      <c r="T21" s="84" t="s">
-        <v>237</v>
-      </c>
-      <c r="U21" s="65" t="s">
-        <v>170</v>
+      <c r="T21" s="83" t="s">
+        <v>224</v>
+      </c>
+      <c r="U21" s="64" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
@@ -3102,23 +3141,23 @@
         <v>147</v>
       </c>
       <c r="D22" s="43" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="F22" s="18"/>
       <c r="G22" s="23" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="H22" s="21">
         <v>20</v>
       </c>
       <c r="I22" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J22" s="25" t="s">
-        <v>233</v>
+        <v>263</v>
       </c>
       <c r="K22" s="29" t="s">
         <v>69</v>
@@ -3138,75 +3177,75 @@
         <v>6</v>
       </c>
       <c r="R22" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="S22" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="S22" s="9" t="s">
-        <v>168</v>
-      </c>
       <c r="T22" s="36" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="U22" s="9" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" s="81" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="66" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" s="80" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="B23" s="67" t="s">
+      <c r="B23" s="66" t="s">
         <v>146</v>
       </c>
-      <c r="C23" s="68" t="s">
+      <c r="C23" s="67" t="s">
         <v>147</v>
       </c>
-      <c r="D23" s="69" t="s">
-        <v>239</v>
-      </c>
-      <c r="E23" s="70" t="s">
+      <c r="D23" s="68" t="s">
+        <v>226</v>
+      </c>
+      <c r="E23" s="69" t="s">
         <v>150</v>
       </c>
-      <c r="F23" s="71"/>
-      <c r="G23" s="72" t="s">
-        <v>241</v>
+      <c r="F23" s="70"/>
+      <c r="G23" s="71" t="s">
+        <v>227</v>
       </c>
       <c r="H23" s="21">
         <v>21</v>
       </c>
-      <c r="I23" s="73" t="s">
+      <c r="I23" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="74" t="s">
-        <v>236</v>
-      </c>
-      <c r="K23" s="75" t="s">
+      <c r="J23" s="73" t="s">
+        <v>257</v>
+      </c>
+      <c r="K23" s="74" t="s">
         <v>69</v>
       </c>
-      <c r="L23" s="76" t="s">
+      <c r="L23" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="M23" s="77" t="s">
+      <c r="M23" s="76" t="s">
         <v>62</v>
       </c>
-      <c r="N23" s="77"/>
-      <c r="O23" s="77"/>
-      <c r="P23" s="79" t="s">
+      <c r="N23" s="76"/>
+      <c r="O23" s="76"/>
+      <c r="P23" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="80">
+      <c r="Q23" s="79">
         <v>6</v>
       </c>
-      <c r="R23" s="80" t="s">
+      <c r="R23" s="79" t="s">
+        <v>166</v>
+      </c>
+      <c r="S23" s="79" t="s">
         <v>167</v>
       </c>
-      <c r="S23" s="80" t="s">
-        <v>168</v>
-      </c>
-      <c r="T23" s="86" t="s">
-        <v>267</v>
-      </c>
-      <c r="U23" s="80" t="s">
-        <v>170</v>
+      <c r="T23" s="85" t="s">
+        <v>249</v>
+      </c>
+      <c r="U23" s="79" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -3220,21 +3259,21 @@
         <v>147</v>
       </c>
       <c r="D24" s="41" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="E24" s="15"/>
       <c r="F24" s="16"/>
       <c r="G24" s="49" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="H24" s="24">
         <v>22</v>
       </c>
       <c r="I24" s="21" t="s">
-        <v>218</v>
-      </c>
-      <c r="J24" s="85" t="s">
-        <v>260</v>
+        <v>211</v>
+      </c>
+      <c r="J24" s="84" t="s">
+        <v>267</v>
       </c>
       <c r="K24" s="27" t="s">
         <v>70</v>
@@ -3245,25 +3284,25 @@
       <c r="M24" s="33"/>
       <c r="N24" s="33"/>
       <c r="O24" s="33" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="P24" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="Q24" s="51" t="s">
-        <v>174</v>
-      </c>
-      <c r="R24" s="51" t="s">
+      <c r="Q24" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="R24" s="50" t="s">
+        <v>160</v>
+      </c>
+      <c r="S24" s="50" t="s">
         <v>161</v>
       </c>
-      <c r="S24" s="51" t="s">
+      <c r="T24" s="50" t="s">
+        <v>212</v>
+      </c>
+      <c r="U24" s="50" t="s">
         <v>162</v>
-      </c>
-      <c r="T24" s="51" t="s">
-        <v>219</v>
-      </c>
-      <c r="U24" s="51" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
@@ -3277,21 +3316,21 @@
         <v>147</v>
       </c>
       <c r="D25" s="43" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="18"/>
       <c r="G25" s="23" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="H25" s="21">
         <v>23</v>
       </c>
       <c r="I25" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J25" s="46" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="K25" s="29" t="s">
         <v>70</v>
@@ -3302,25 +3341,25 @@
       <c r="M25" s="33"/>
       <c r="N25" s="33"/>
       <c r="O25" s="37" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="P25" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q25" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="R25" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="S25" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="S25" s="9" t="s">
+      <c r="T25" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="U25" s="9" t="s">
         <v>162</v>
-      </c>
-      <c r="T25" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="U25" s="9" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
@@ -3334,21 +3373,21 @@
         <v>147</v>
       </c>
       <c r="D26" s="43" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="18"/>
       <c r="G26" s="23" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="H26" s="21">
         <v>24</v>
       </c>
       <c r="I26" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J26" s="46" t="s">
-        <v>240</v>
+        <v>258</v>
       </c>
       <c r="K26" s="29" t="s">
         <v>70</v>
@@ -3359,139 +3398,139 @@
       <c r="M26" s="33"/>
       <c r="N26" s="33"/>
       <c r="O26" s="32" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="P26" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q26" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="R26" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="S26" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="S26" s="9" t="s">
+      <c r="T26" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="U26" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="T26" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="U26" s="9" t="s">
-        <v>163</v>
-      </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="52" t="s">
+      <c r="A27" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="53" t="s">
+      <c r="B27" s="52" t="s">
         <v>146</v>
       </c>
-      <c r="C27" s="54" t="s">
+      <c r="C27" s="53" t="s">
         <v>147</v>
       </c>
-      <c r="D27" s="82" t="s">
-        <v>217</v>
-      </c>
-      <c r="E27" s="83"/>
-      <c r="F27" s="57"/>
-      <c r="G27" s="58" t="s">
-        <v>225</v>
+      <c r="D27" s="81" t="s">
+        <v>210</v>
+      </c>
+      <c r="E27" s="82"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="57" t="s">
+        <v>220</v>
       </c>
       <c r="H27" s="24">
         <v>25</v>
       </c>
-      <c r="I27" s="59" t="s">
-        <v>166</v>
-      </c>
-      <c r="J27" s="87" t="s">
-        <v>261</v>
-      </c>
-      <c r="K27" s="60" t="s">
+      <c r="I27" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="J27" s="86" t="s">
+        <v>243</v>
+      </c>
+      <c r="K27" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="L27" s="61" t="s">
+      <c r="L27" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="M27" s="62"/>
-      <c r="N27" s="62"/>
-      <c r="O27" s="63" t="s">
-        <v>227</v>
-      </c>
-      <c r="P27" s="64" t="s">
+      <c r="M27" s="61"/>
+      <c r="N27" s="61"/>
+      <c r="O27" s="62" t="s">
+        <v>219</v>
+      </c>
+      <c r="P27" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="Q27" s="65" t="s">
-        <v>174</v>
-      </c>
-      <c r="R27" s="65" t="s">
-        <v>161</v>
-      </c>
-      <c r="S27" s="65" t="s">
-        <v>195</v>
-      </c>
-      <c r="T27" s="65" t="s">
-        <v>228</v>
-      </c>
-      <c r="U27" s="65" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" s="81" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="66" t="s">
+      <c r="Q27" s="64" t="s">
+        <v>172</v>
+      </c>
+      <c r="R27" s="64" t="s">
+        <v>160</v>
+      </c>
+      <c r="S27" s="64" t="s">
+        <v>190</v>
+      </c>
+      <c r="T27" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="U27" s="64" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" s="80" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="B28" s="67" t="s">
+      <c r="B28" s="66" t="s">
         <v>146</v>
       </c>
-      <c r="C28" s="68" t="s">
+      <c r="C28" s="67" t="s">
         <v>147</v>
       </c>
-      <c r="D28" s="69" t="s">
-        <v>217</v>
-      </c>
-      <c r="E28" s="70"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="72" t="s">
-        <v>229</v>
+      <c r="D28" s="68" t="s">
+        <v>210</v>
+      </c>
+      <c r="E28" s="69"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="71" t="s">
+        <v>221</v>
       </c>
       <c r="H28" s="21">
         <v>26</v>
       </c>
-      <c r="I28" s="73" t="s">
-        <v>166</v>
-      </c>
-      <c r="J28" s="88" t="s">
-        <v>230</v>
-      </c>
-      <c r="K28" s="75" t="s">
+      <c r="I28" s="72" t="s">
+        <v>165</v>
+      </c>
+      <c r="J28" s="87" t="s">
+        <v>259</v>
+      </c>
+      <c r="K28" s="74" t="s">
         <v>70</v>
       </c>
-      <c r="L28" s="76" t="s">
+      <c r="L28" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="M28" s="77"/>
-      <c r="N28" s="77"/>
-      <c r="O28" s="77" t="s">
-        <v>226</v>
-      </c>
-      <c r="P28" s="79" t="s">
+      <c r="M28" s="76"/>
+      <c r="N28" s="76"/>
+      <c r="O28" s="76" t="s">
+        <v>218</v>
+      </c>
+      <c r="P28" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="Q28" s="80" t="s">
-        <v>174</v>
-      </c>
-      <c r="R28" s="80" t="s">
-        <v>161</v>
-      </c>
-      <c r="S28" s="80" t="s">
-        <v>195</v>
-      </c>
-      <c r="T28" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="U28" s="80" t="s">
-        <v>197</v>
+      <c r="Q28" s="79" t="s">
+        <v>172</v>
+      </c>
+      <c r="R28" s="79" t="s">
+        <v>160</v>
+      </c>
+      <c r="S28" s="79" t="s">
+        <v>190</v>
+      </c>
+      <c r="T28" s="79" t="s">
+        <v>222</v>
+      </c>
+      <c r="U28" s="79" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -3505,21 +3544,21 @@
         <v>147</v>
       </c>
       <c r="D29" s="41" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="E29" s="15"/>
       <c r="F29" s="16"/>
       <c r="G29" s="49" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
       <c r="H29" s="21">
         <v>27</v>
       </c>
       <c r="I29" s="21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J29" s="49" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
       <c r="K29" s="27" t="s">
         <v>69</v>
@@ -3533,11 +3572,11 @@
       <c r="P29" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="Q29" s="51"/>
-      <c r="R29" s="51"/>
-      <c r="S29" s="51"/>
-      <c r="T29" s="51"/>
-      <c r="U29" s="51"/>
+      <c r="Q29" s="50"/>
+      <c r="R29" s="50"/>
+      <c r="S29" s="50"/>
+      <c r="T29" s="50"/>
+      <c r="U29" s="50"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="42" t="s">
@@ -3550,21 +3589,21 @@
         <v>147</v>
       </c>
       <c r="D30" s="43" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="18"/>
       <c r="G30" s="23" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
       <c r="H30" s="21">
         <v>28</v>
       </c>
       <c r="I30" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J30" s="25" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
       <c r="K30" s="29" t="s">
         <v>69</v>
@@ -3584,64 +3623,64 @@
         <v>6</v>
       </c>
       <c r="R30" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="S30" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="S30" s="9" t="s">
-        <v>168</v>
-      </c>
       <c r="T30" s="36" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="U30" s="9" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" s="81" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="66" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" s="80" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="67" t="s">
+      <c r="B31" s="66" t="s">
         <v>146</v>
       </c>
-      <c r="C31" s="68" t="s">
+      <c r="C31" s="67" t="s">
         <v>147</v>
       </c>
-      <c r="D31" s="69" t="s">
-        <v>262</v>
-      </c>
-      <c r="E31" s="70"/>
-      <c r="F31" s="71"/>
-      <c r="G31" s="92" t="s">
-        <v>242</v>
+      <c r="D31" s="68" t="s">
+        <v>244</v>
+      </c>
+      <c r="E31" s="69"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="91" t="s">
+        <v>228</v>
       </c>
       <c r="H31" s="24">
         <v>29</v>
       </c>
-      <c r="I31" s="73" t="s">
-        <v>166</v>
-      </c>
-      <c r="J31" s="74" t="s">
-        <v>243</v>
-      </c>
-      <c r="K31" s="75" t="s">
+      <c r="I31" s="72" t="s">
+        <v>165</v>
+      </c>
+      <c r="J31" s="73" t="s">
+        <v>268</v>
+      </c>
+      <c r="K31" s="74" t="s">
         <v>70</v>
       </c>
-      <c r="L31" s="76" t="s">
+      <c r="L31" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="M31" s="93" t="s">
+      <c r="M31" s="92" t="s">
         <v>63</v>
       </c>
-      <c r="N31" s="77"/>
-      <c r="O31" s="77"/>
-      <c r="P31" s="94" t="s">
+      <c r="N31" s="76"/>
+      <c r="O31" s="76"/>
+      <c r="P31" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="Q31" s="95"/>
-      <c r="R31" s="96"/>
-      <c r="S31" s="96"/>
-      <c r="T31" s="96"/>
-      <c r="U31" s="97"/>
+      <c r="Q31" s="94"/>
+      <c r="R31" s="95"/>
+      <c r="S31" s="95"/>
+      <c r="T31" s="95"/>
+      <c r="U31" s="96"/>
     </row>
     <row r="32" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A32" s="38"/>
@@ -3660,11 +3699,11 @@
       <c r="N32" s="33"/>
       <c r="O32" s="33"/>
       <c r="P32" s="31"/>
-      <c r="Q32" s="89"/>
-      <c r="R32" s="90"/>
-      <c r="S32" s="90"/>
-      <c r="T32" s="90"/>
-      <c r="U32" s="91"/>
+      <c r="Q32" s="88"/>
+      <c r="R32" s="89"/>
+      <c r="S32" s="89"/>
+      <c r="T32" s="89"/>
+      <c r="U32" s="90"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="42"/>

</xml_diff>